<commit_message>
adding script to look at flanker behavioral data
</commit_message>
<xml_diff>
--- a/data/FujitsuTiers.xlsx
+++ b/data/FujitsuTiers.xlsx
@@ -20,26 +20,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t xml:space="preserve">Group</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Before dir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After dir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Before Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nd epoch is bad here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11052018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bad channels here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09062018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st epoch is bad here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11142018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11122018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11012018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11132018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11022018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11092018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11072018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -55,6 +108,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,9 +158,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -121,15 +196,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -139,6 +216,18 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -147,6 +236,13 @@
       <c r="B2" s="0" t="n">
         <v>32960218</v>
       </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="n">
+        <v>11062018</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -155,6 +251,13 @@
       <c r="B3" s="0" t="n">
         <v>31970318</v>
       </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4" t="n">
+        <v>11052018</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -163,6 +266,13 @@
       <c r="B4" s="0" t="n">
         <v>32950518</v>
       </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4" t="n">
+        <v>11062018</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -171,6 +281,13 @@
       <c r="B5" s="0" t="n">
         <v>32950318</v>
       </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -179,6 +296,15 @@
       <c r="B6" s="0" t="n">
         <v>31960118</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>11062018</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -187,6 +313,12 @@
       <c r="B7" s="0" t="n">
         <v>31970218</v>
       </c>
+      <c r="C7" s="4" t="n">
+        <v>9072018</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>11072018</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -195,6 +327,10 @@
       <c r="B8" s="0" t="n">
         <v>319100118</v>
       </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -203,6 +339,10 @@
       <c r="B9" s="0" t="n">
         <v>319110218</v>
       </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4" t="n">
+        <v>11072018</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -211,6 +351,10 @@
       <c r="B10" s="0" t="n">
         <v>32960418</v>
       </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -219,21 +363,27 @@
       <c r="B11" s="0" t="n">
         <v>319110118</v>
       </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>31950418</v>
-      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>310910318</v>
+        <v>31950418</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>9052018</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>11142018</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -241,7 +391,11 @@
         <v>2</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>32960318</v>
+        <v>310910318</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -249,7 +403,11 @@
         <v>2</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>32970418</v>
+        <v>32960318</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -257,7 +415,11 @@
         <v>2</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>3209110318</v>
+        <v>32970418</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -265,7 +427,11 @@
         <v>2</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>3209120218</v>
+        <v>3209110318</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -273,7 +439,11 @@
         <v>2</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>319100418</v>
+        <v>3209120218</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -281,7 +451,11 @@
         <v>2</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>31970118</v>
+        <v>319100418</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -289,7 +463,11 @@
         <v>2</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>32050118</v>
+        <v>31970118</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -297,7 +475,11 @@
         <v>2</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>31950218</v>
+        <v>32050118</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -305,24 +487,48 @@
         <v>2</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>3109120318</v>
+        <v>31950218</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>3109120318</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B25" s="0" t="n">
         <v>32910218</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B26" s="0" t="n">
         <v>3109120118</v>
       </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
dding sanity check of RT for Intheon, etc.dding sanity check of RT for Intheon, etc.
</commit_message>
<xml_diff>
--- a/data/FujitsuTiers.xlsx
+++ b/data/FujitsuTiers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t xml:space="preserve">Group</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">After notes</t>
   </si>
   <si>
+    <t xml:space="preserve">General notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">2nd epoch is bad here</t>
   </si>
   <si>
@@ -52,9 +55,6 @@
     <t xml:space="preserve">bad channels here</t>
   </si>
   <si>
-    <t xml:space="preserve">09062018</t>
-  </si>
-  <si>
     <t xml:space="preserve">1st epoch is bad here</t>
   </si>
   <si>
@@ -64,19 +64,37 @@
     <t xml:space="preserve">11122018</t>
   </si>
   <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11132018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11022018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suhas; also files in untitled directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11092018</t>
+  </si>
+  <si>
     <t xml:space="preserve">11012018</t>
   </si>
   <si>
-    <t xml:space="preserve">11132018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11022018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11092018</t>
-  </si>
-  <si>
     <t xml:space="preserve">11072018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winnie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excluded (motor control issue)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excluded (non-FLA employee)</t>
   </si>
 </sst>
 </file>
@@ -87,7 +105,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -108,12 +126,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,7 +170,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -167,15 +179,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,10 +200,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -216,10 +220,10 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
@@ -228,6 +232,9 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -236,12 +243,12 @@
       <c r="B2" s="0" t="n">
         <v>32960218</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="n">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="n">
         <v>11062018</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -251,12 +258,12 @@
       <c r="B3" s="0" t="n">
         <v>31970318</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4" t="n">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="n">
         <v>11052018</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -266,12 +273,12 @@
       <c r="B4" s="0" t="n">
         <v>32950518</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4" t="n">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="n">
         <v>11062018</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -281,12 +288,12 @@
       <c r="B5" s="0" t="n">
         <v>32950318</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -296,10 +303,10 @@
       <c r="B6" s="0" t="n">
         <v>31960118</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4" t="n">
+      <c r="C6" s="2" t="n">
+        <v>9062018</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>11062018</v>
       </c>
       <c r="E6" s="0" t="s">
@@ -313,10 +320,10 @@
       <c r="B7" s="0" t="n">
         <v>31970218</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="2" t="n">
         <v>9072018</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="2" t="n">
         <v>11072018</v>
       </c>
     </row>
@@ -327,8 +334,8 @@
       <c r="B8" s="0" t="n">
         <v>319100118</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -339,8 +346,8 @@
       <c r="B9" s="0" t="n">
         <v>319110218</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4" t="n">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="n">
         <v>11072018</v>
       </c>
     </row>
@@ -351,8 +358,8 @@
       <c r="B10" s="0" t="n">
         <v>32960418</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -363,14 +370,14 @@
       <c r="B11" s="0" t="n">
         <v>319110118</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
-        <v>14</v>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="n">
+        <v>11052018</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -379,11 +386,14 @@
       <c r="B13" s="0" t="n">
         <v>31950418</v>
       </c>
-      <c r="C13" s="4" t="n">
+      <c r="C13" s="2" t="n">
         <v>9052018</v>
       </c>
-      <c r="D13" s="4" t="n">
+      <c r="D13" s="2" t="n">
         <v>11142018</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -393,9 +403,14 @@
       <c r="B14" s="0" t="n">
         <v>310910318</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
+      <c r="C14" s="2" t="n">
+        <v>9102018</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -405,9 +420,17 @@
       <c r="B15" s="0" t="n">
         <v>32960318</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
+      <c r="C15" s="2" t="n">
+        <v>9062018</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,9 +440,14 @@
       <c r="B16" s="0" t="n">
         <v>32970418</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
+      <c r="C16" s="2" t="n">
+        <v>9072018</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -429,9 +457,14 @@
       <c r="B17" s="0" t="n">
         <v>3209110318</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
-        <v>17</v>
+      <c r="C17" s="2" t="n">
+        <v>9112018</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -441,8 +474,13 @@
       <c r="B18" s="0" t="n">
         <v>3209120218</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
+      <c r="C18" s="2" t="n">
+        <v>9122018</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>14</v>
       </c>
     </row>
@@ -453,9 +491,14 @@
       <c r="B19" s="0" t="n">
         <v>319100418</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3" t="s">
+      <c r="C19" s="2" t="n">
+        <v>9102018</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -465,9 +508,14 @@
       <c r="B20" s="0" t="n">
         <v>31970118</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
-        <v>17</v>
+      <c r="C20" s="2" t="n">
+        <v>9072018</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,9 +525,17 @@
       <c r="B21" s="0" t="n">
         <v>32050118</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3" t="s">
-        <v>18</v>
+      <c r="C21" s="2" t="n">
+        <v>9052018</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,9 +545,14 @@
       <c r="B22" s="0" t="n">
         <v>31950218</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3" t="s">
+      <c r="C22" s="2" t="n">
+        <v>9052018</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,14 +562,16 @@
       <c r="B23" s="0" t="n">
         <v>3109120318</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
-        <v>18</v>
+      <c r="C23" s="2" t="n">
+        <v>9122018</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -517,8 +580,13 @@
       <c r="B25" s="0" t="n">
         <v>32910218</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="n">
+        <v>11122018</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -527,8 +595,13 @@
       <c r="B26" s="0" t="n">
         <v>3109120118</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
FujitsuTiers.xlsx - color coding (there was a color coded version somewhere...maybe Dropbox)
view_neuroscale_multiple_grp_report.m - writing out bands and ratios to Excel using support/intheon_to_xlsx.m
</commit_message>
<xml_diff>
--- a/data/FujitsuTiers.xlsx
+++ b/data/FujitsuTiers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suhas\Desktop\prjs\cognitive_measures\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4682FFCD-606A-445F-934B-C72A3AB6237A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703D4C3F-F5A9-4BC5-BD7F-D771F4A49508}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="7824" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5508" yWindow="1668" windowWidth="23040" windowHeight="7824" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Group</t>
   </si>
@@ -103,21 +103,37 @@
   </si>
   <si>
     <t>Excluded (non-FLA employee)</t>
+  </si>
+  <si>
+    <t>DANA file lacks markers.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,12 +142,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -139,24 +167,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,556 +533,559 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.5546875"/>
-    <col min="3" max="4" width="11.5546875" style="1"/>
-    <col min="5" max="1025" width="11.5546875"/>
+    <col min="1" max="2" width="11.5546875" style="2"/>
+    <col min="3" max="4" width="11.5546875" style="12"/>
+    <col min="5" max="1025" width="11.5546875" style="2"/>
+    <col min="1026" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>32960218</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>9062018</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="13">
         <v>11062018</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>31970318</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>9072018</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>11052018</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>32950518</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>9052018</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>11062018</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>32950318</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>9052018</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>31960118</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>9062018</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>11062018</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>31970218</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>9072018</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>11072018</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>319100118</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>9102018</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>319110218</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="14">
         <v>9112018</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="13">
         <v>11072018</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>1</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>32960418</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>9062018</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>1</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>319110118</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>9112018</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="13">
         <v>11052018</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>2</v>
-      </c>
-      <c r="B12" s="4">
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>2</v>
+      </c>
+      <c r="B12" s="6">
         <v>31950418</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="7">
         <v>9052018</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="7">
         <v>11142018</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>2</v>
-      </c>
-      <c r="B13" s="4">
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>2</v>
+      </c>
+      <c r="B13" s="6">
         <v>310910318</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="7">
         <v>9102018</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>2</v>
+      </c>
+      <c r="B14" s="6">
         <v>32960318</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="7">
         <v>9062018</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>2</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>2</v>
+      </c>
+      <c r="B15" s="6">
         <v>32970418</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="7">
         <v>9072018</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>2</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>2</v>
+      </c>
+      <c r="B16" s="6">
         <v>3209110318</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="7">
         <v>9112018</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>2</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>2</v>
+      </c>
+      <c r="B17" s="6">
         <v>3209120218</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="7">
         <v>9122018</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>2</v>
-      </c>
-      <c r="B18" s="4">
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>2</v>
+      </c>
+      <c r="B18" s="6">
         <v>319100418</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="7">
         <v>9102018</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>2</v>
-      </c>
-      <c r="B19" s="2">
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>2</v>
+      </c>
+      <c r="B19" s="6">
         <v>31970118</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="7">
         <v>9072018</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>2</v>
-      </c>
-      <c r="B20" s="4">
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>2</v>
+      </c>
+      <c r="B20" s="6">
         <v>32050118</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="7">
         <v>9052018</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4" t="s">
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>2</v>
-      </c>
-      <c r="B21" s="2">
+    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>2</v>
+      </c>
+      <c r="B21" s="6">
         <v>31950218</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="7">
         <v>9052018</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>2</v>
-      </c>
-      <c r="B22" s="2">
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>2</v>
+      </c>
+      <c r="B22" s="6">
         <v>3109120318</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="7">
         <v>9122018</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2" t="s">
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+    <row r="23" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
         <v>3</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="9">
         <v>32910218</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="9">
         <v>9102018</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="10">
         <v>11122018</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+    </row>
+    <row r="24" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
         <v>3</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="9">
         <v>3109120118</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="9">
         <v>9122018</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="10">
         <v>-1</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
dump of DANA and visual arrest group data in reasonable Excel format
various renames
</commit_message>
<xml_diff>
--- a/data/FujitsuTiers.xlsx
+++ b/data/FujitsuTiers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suhas\Desktop\prjs\cognitive_measures\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703D4C3F-F5A9-4BC5-BD7F-D771F4A49508}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494D18E3-7D41-4FB8-A2C0-67DBE4312905}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5508" yWindow="1668" windowWidth="23040" windowHeight="7824" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="1632" windowWidth="23040" windowHeight="7824" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Group</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>DANA file lacks markers.</t>
+  </si>
+  <si>
+    <t>Asked for an individual report</t>
+  </si>
+  <si>
+    <t>Wants individual report</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -186,25 +195,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -531,21 +536,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="2"/>
-    <col min="3" max="4" width="11.5546875" style="12"/>
-    <col min="5" max="1025" width="11.5546875" style="2"/>
-    <col min="1026" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="2" width="11.5546875" style="1"/>
+    <col min="3" max="4" width="11.5546875" style="8"/>
+    <col min="5" max="5" width="11.5546875" style="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="1026" width="11.5546875" style="1"/>
+    <col min="1027" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,529 +566,411 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="M1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
         <v>32960218</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>9062018</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="9">
         <v>11062018</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3">
+    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
         <v>31970318</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>9072018</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>11052018</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3">
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
         <v>32950518</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>9052018</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>11062018</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3">
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
         <v>32950318</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>9052018</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
         <v>31960118</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>9062018</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>11062018</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
         <v>31970218</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>9072018</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>11072018</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3">
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
         <v>319100118</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>9102018</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3">
+    </row>
+    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2">
         <v>319110218</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="10">
         <v>9112018</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="9">
         <v>11072018</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3" t="s">
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3">
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
         <v>32960418</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>9062018</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>1</v>
-      </c>
-      <c r="B11" s="3">
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2">
         <v>319110118</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>9112018</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="9">
         <v>11052018</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3" t="s">
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>2</v>
-      </c>
-      <c r="B12" s="6">
+    </row>
+    <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4">
         <v>31950418</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>9052018</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>11142018</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>2</v>
-      </c>
-      <c r="B13" s="6">
+      <c r="E12" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>2</v>
+      </c>
+      <c r="B13" s="4">
         <v>310910318</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <v>9102018</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>2</v>
-      </c>
-      <c r="B14" s="6">
+      <c r="E13" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4">
         <v>32960318</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <v>9062018</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="F14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>2</v>
-      </c>
-      <c r="B15" s="6">
+    </row>
+    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4">
         <v>32970418</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="5">
         <v>9072018</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>2</v>
-      </c>
-      <c r="B16" s="6">
+    </row>
+    <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4">
         <v>3209110318</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="5">
         <v>9112018</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>2</v>
-      </c>
-      <c r="B17" s="6">
+    </row>
+    <row r="17" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4">
         <v>3209120218</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="5">
         <v>9122018</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>2</v>
-      </c>
-      <c r="B18" s="6">
+    </row>
+    <row r="18" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>2</v>
+      </c>
+      <c r="B18" s="4">
         <v>319100418</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="5">
         <v>9102018</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>2</v>
-      </c>
-      <c r="B19" s="6">
+      <c r="E18" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>2</v>
+      </c>
+      <c r="B19" s="4">
         <v>31970118</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="5">
         <v>9072018</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>2</v>
-      </c>
-      <c r="B20" s="6">
+    </row>
+    <row r="20" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>2</v>
+      </c>
+      <c r="B20" s="4">
         <v>32050118</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="5">
         <v>9052018</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6" t="s">
+      <c r="L20" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>2</v>
-      </c>
-      <c r="B21" s="6">
+    <row r="21" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>2</v>
+      </c>
+      <c r="B21" s="4">
         <v>31950218</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="5">
         <v>9052018</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>2</v>
-      </c>
-      <c r="B22" s="6">
+    </row>
+    <row r="22" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>2</v>
+      </c>
+      <c r="B22" s="4">
         <v>3109120318</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="5">
         <v>9122018</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6" t="s">
+      <c r="L22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+    <row r="23" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
         <v>3</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="6">
         <v>32910218</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="6">
         <v>9102018</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="7">
         <v>11122018</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+    </row>
+    <row r="24" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
         <v>3</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="6">
         <v>3109120118</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="6">
         <v>9122018</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="7">
         <v>-1</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="F24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
saving out ind. reports w/ view_neuroscale_multiple_grp_report__display.m (bad name)
making fig's in make_fj_individ_reports.m
</commit_message>
<xml_diff>
--- a/data/FujitsuTiers.xlsx
+++ b/data/FujitsuTiers.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suhas\Desktop\prjs\cognitive_measures\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494D18E3-7D41-4FB8-A2C0-67DBE4312905}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A801808C-BD7E-47B9-A1DE-56E1392A2E55}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1632" windowWidth="23040" windowHeight="7824" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sort by ID" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
   <si>
     <t>Group</t>
   </si>
@@ -538,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="A1:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -980,4 +981,405 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AFF2F8D-CE60-43ED-87CB-731B31608D1B}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4">
+        <v>31950218</v>
+      </c>
+      <c r="C2" s="5">
+        <v>9052018</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>31950418</v>
+      </c>
+      <c r="C3" s="5">
+        <v>9052018</v>
+      </c>
+      <c r="D3" s="5">
+        <v>11142018</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>31960118</v>
+      </c>
+      <c r="C4" s="3">
+        <v>9062018</v>
+      </c>
+      <c r="D4" s="3">
+        <v>11062018</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
+        <v>31970118</v>
+      </c>
+      <c r="C5" s="5">
+        <v>9072018</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>31970218</v>
+      </c>
+      <c r="C6" s="3">
+        <v>9072018</v>
+      </c>
+      <c r="D6" s="3">
+        <v>11072018</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>31970318</v>
+      </c>
+      <c r="C7" s="2">
+        <v>9072018</v>
+      </c>
+      <c r="D7" s="3">
+        <v>11052018</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4">
+        <v>32050118</v>
+      </c>
+      <c r="C8" s="5">
+        <v>9052018</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>3</v>
+      </c>
+      <c r="B9" s="6">
+        <v>32910218</v>
+      </c>
+      <c r="C9" s="6">
+        <v>9102018</v>
+      </c>
+      <c r="D9" s="7">
+        <v>11122018</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>32950318</v>
+      </c>
+      <c r="C10" s="2">
+        <v>9052018</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2">
+        <v>32950518</v>
+      </c>
+      <c r="C11" s="2">
+        <v>9052018</v>
+      </c>
+      <c r="D11" s="3">
+        <v>11062018</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>32960218</v>
+      </c>
+      <c r="C12" s="2">
+        <v>9062018</v>
+      </c>
+      <c r="D12" s="9">
+        <v>11062018</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>2</v>
+      </c>
+      <c r="B13" s="4">
+        <v>32960318</v>
+      </c>
+      <c r="C13" s="5">
+        <v>9062018</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2">
+        <v>32960418</v>
+      </c>
+      <c r="C14" s="2">
+        <v>9062018</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4">
+        <v>32970418</v>
+      </c>
+      <c r="C15" s="5">
+        <v>9072018</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4">
+        <v>310910318</v>
+      </c>
+      <c r="C16" s="5">
+        <v>9102018</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2">
+        <v>319100118</v>
+      </c>
+      <c r="C17" s="2">
+        <v>9102018</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>2</v>
+      </c>
+      <c r="B18" s="4">
+        <v>319100418</v>
+      </c>
+      <c r="C18" s="5">
+        <v>9102018</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2">
+        <v>319110118</v>
+      </c>
+      <c r="C19" s="2">
+        <v>9112018</v>
+      </c>
+      <c r="D19" s="9">
+        <v>11052018</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2">
+        <v>319110218</v>
+      </c>
+      <c r="C20" s="10">
+        <v>9112018</v>
+      </c>
+      <c r="D20" s="9">
+        <v>11072018</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>3</v>
+      </c>
+      <c r="B21" s="6">
+        <v>3109120118</v>
+      </c>
+      <c r="C21" s="6">
+        <v>9122018</v>
+      </c>
+      <c r="D21" s="7">
+        <v>-1</v>
+      </c>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>2</v>
+      </c>
+      <c r="B22" s="4">
+        <v>3109120318</v>
+      </c>
+      <c r="C22" s="5">
+        <v>9122018</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>2</v>
+      </c>
+      <c r="B23" s="4">
+        <v>3209110318</v>
+      </c>
+      <c r="C23" s="5">
+        <v>9112018</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>2</v>
+      </c>
+      <c r="B24" s="4">
+        <v>3209120218</v>
+      </c>
+      <c r="C24" s="5">
+        <v>9122018</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="4"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E24">
+    <sortCondition ref="B2:B24"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
checkpointing before being able to get an inidivudal report w/o an after (just a before)
data/FujitsuTiers.xlsx - just labeled first sheet
</commit_message>
<xml_diff>
--- a/data/FujitsuTiers.xlsx
+++ b/data/FujitsuTiers.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suhas\Desktop\prjs\cognitive_measures\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5F5773-EA50-4BC1-90CA-A129A5A07158}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9153A0E5-6509-4854-9DE0-13EB6622154C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="384" windowWidth="23040" windowHeight="10548" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sort by Tier" sheetId="1" r:id="rId1"/>
     <sheet name="Sort by ID" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="A1:E24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1066,7 +1066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AFF2F8D-CE60-43ED-87CB-731B31608D1B}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>